<commit_message>
Updated templates for better interpretability
</commit_message>
<xml_diff>
--- a/jojoAttempt2/media/media/team-first-msexcel.xlsx
+++ b/jojoAttempt2/media/media/team-first-msexcel.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malolemagueresse/Documents/GitHub/teamFormation/jojoAttempt2/media/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8102107A-2EC9-3747-BC3B-36EA4B544D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64158FF2-948B-F442-A430-6E1178615238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{12FBB817-7B2B-EB4B-9728-877CC806AFD9}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{12FBB817-7B2B-EB4B-9728-877CC806AFD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="User Guide" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="CSV_Example" localSheetId="0">Data!$A$1:$F$49</definedName>
@@ -74,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
   <si>
     <t>Last Name</t>
   </si>
@@ -82,12 +81,6 @@
     <t>Email Address</t>
   </si>
   <si>
-    <t>Employment Status</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>First name</t>
   </si>
   <si>
@@ -220,10 +213,16 @@
     <t>y</t>
   </si>
   <si>
-    <t>How familiar are you with Data Science?</t>
-  </si>
-  <si>
-    <t>Template User Guide</t>
+    <t>How familiar are you with Data Science?
+1 = Have not attended a DS class, 2 = Attended 1 or 2 DS classes, 3 = Attended 3+ DS classes</t>
+  </si>
+  <si>
+    <t>Employment Status
+1 = Not employed, 2 = Part-time, 3 = Full-time professional</t>
+  </si>
+  <si>
+    <t>Teamwork style
+1 = Careful, 2 = Clutch, 3 = Acceleration</t>
   </si>
 </sst>
 </file>
@@ -270,7 +269,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,21 +592,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ED3309-03E4-BC47-A16D-21374FA961F7}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -614,24 +615,24 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -645,13 +646,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -665,13 +666,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -685,13 +686,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -705,13 +706,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -725,13 +726,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -745,13 +746,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -765,13 +766,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -785,13 +786,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -800,18 +801,18 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -825,13 +826,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -845,13 +846,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -865,13 +866,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -885,13 +886,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -905,13 +906,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -925,13 +926,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -945,13 +946,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -965,13 +966,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -985,13 +986,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1005,13 +1006,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1025,13 +1026,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1045,13 +1046,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1060,18 +1061,18 @@
         <v>3</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1085,13 +1086,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1105,13 +1106,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1125,13 +1126,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1145,13 +1146,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1165,13 +1166,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1185,13 +1186,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1200,18 +1201,18 @@
         <v>3</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1225,13 +1226,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1245,13 +1246,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1260,18 +1261,18 @@
         <v>3</v>
       </c>
       <c r="F33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1285,13 +1286,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1305,13 +1306,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1325,13 +1326,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1345,13 +1346,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1365,13 +1366,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1380,18 +1381,18 @@
         <v>3</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -1405,13 +1406,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1425,13 +1426,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1445,13 +1446,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -1465,13 +1466,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -1485,13 +1486,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1505,13 +1506,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D46">
         <v>3</v>
@@ -1520,18 +1521,18 @@
         <v>3</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -1545,13 +1546,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -1565,13 +1566,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1582,31 +1583,6 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E93A207-EB85-0249-A432-A9E6AF8EEA5D}">
-  <dimension ref="B2:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>